<commit_message>
jdre-12/03/2015-Se modifico la BITACORA.xlsx
</commit_message>
<xml_diff>
--- a/ afgmx/AFGMX/ADMON_DEL_PROYECTO/BITACORAS/2015/CUAT_1_ENER_ABR/PARCIAL_3/BITACORA.xlsx
+++ b/ afgmx/AFGMX/ADMON_DEL_PROYECTO/BITACORAS/2015/CUAT_1_ENER_ABR/PARCIAL_3/BITACORA.xlsx
@@ -194,9 +194,6 @@
     <t>Base de datos para aplicaciones</t>
   </si>
   <si>
-    <t>Verificación de nuevas actividades e integración de procesos</t>
-  </si>
-  <si>
     <t>Finalizado</t>
   </si>
   <si>
@@ -207,6 +204,9 @@
   </si>
   <si>
     <t>Juan Diego Romero Espinoza, Carlos Enrique Hernandez Jiménez e Ing. Ramiro Alcazar Magaña</t>
+  </si>
+  <si>
+    <t>Incripción a posible y acuerdos para el desarrollo del software</t>
   </si>
 </sst>
 </file>
@@ -1293,15 +1293,45 @@
     </xf>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="54" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="53" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="46" fillId="22" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="54" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1314,23 +1344,14 @@
     <xf numFmtId="0" fontId="23" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1341,71 +1362,50 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="24" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="18" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="24" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="18" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="53" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1926,46 +1926,46 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="43"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="40"/>
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="43"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="40"/>
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="43"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="40"/>
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1988,13 +1988,13 @@
       <c r="C6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
@@ -2006,13 +2006,13 @@
       <c r="C7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
@@ -2024,13 +2024,13 @@
       <c r="C8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -2042,13 +2042,13 @@
       <c r="C9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
       <c r="I9" s="15"/>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
@@ -2060,13 +2060,13 @@
       <c r="C10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="36">
+      <c r="D10" s="44">
         <v>1</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
@@ -2078,13 +2078,13 @@
       <c r="C11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
@@ -2110,11 +2110,11 @@
       <c r="C13" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
       <c r="I13" s="15"/>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
@@ -2126,13 +2126,13 @@
       <c r="C14" s="26">
         <v>1</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
@@ -2144,13 +2144,13 @@
       <c r="C15" s="26">
         <v>2</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
@@ -2162,13 +2162,13 @@
       <c r="C16" s="26">
         <v>3</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
       <c r="I16" s="15"/>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
@@ -2180,13 +2180,13 @@
       <c r="C17" s="26">
         <v>4</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
@@ -2198,13 +2198,13 @@
       <c r="C18" s="26">
         <v>5</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
@@ -2216,11 +2216,11 @@
       <c r="C19" s="26">
         <v>6</v>
       </c>
-      <c r="D19" s="34"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
@@ -2242,11 +2242,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B2:K4"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="D9:H9"/>
     <mergeCell ref="D16:H16"/>
     <mergeCell ref="D17:H17"/>
     <mergeCell ref="D18:H18"/>
@@ -2256,6 +2251,11 @@
     <mergeCell ref="D13:H13"/>
     <mergeCell ref="D14:H14"/>
     <mergeCell ref="D15:H15"/>
+    <mergeCell ref="B2:K4"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="D9:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2267,7 +2267,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2311,42 +2311,42 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="71"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="53"/>
       <c r="J3" s="19"/>
       <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
-      <c r="B4" s="69"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="71"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="53"/>
       <c r="J4" s="19"/>
       <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="71"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="53"/>
       <c r="J5" s="19"/>
       <c r="K5" s="7"/>
     </row>
@@ -2407,28 +2407,28 @@
     </row>
     <row r="9" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
-      <c r="B9" s="66">
+      <c r="B9" s="35">
         <v>1</v>
       </c>
-      <c r="C9" s="67">
+      <c r="C9" s="36">
         <v>42074</v>
       </c>
-      <c r="D9" s="65" t="s">
+      <c r="D9" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="66" t="s">
+      <c r="F9" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="G9" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="H9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" s="68"/>
+      <c r="I9" s="37"/>
       <c r="J9" s="2"/>
       <c r="K9" s="15"/>
     </row>
@@ -2657,74 +2657,74 @@
     </row>
     <row r="2" spans="1:21" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
-      <c r="U2" s="49"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="56"/>
     </row>
     <row r="3" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="48"/>
-      <c r="S3" s="48"/>
-      <c r="T3" s="48"/>
-      <c r="U3" s="49"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="55"/>
+      <c r="T3" s="55"/>
+      <c r="U3" s="56"/>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48"/>
-      <c r="O4" s="48"/>
-      <c r="P4" s="48"/>
-      <c r="Q4" s="48"/>
-      <c r="R4" s="48"/>
-      <c r="S4" s="48"/>
-      <c r="T4" s="48"/>
-      <c r="U4" s="49"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="55"/>
+      <c r="L4" s="55"/>
+      <c r="M4" s="55"/>
+      <c r="N4" s="55"/>
+      <c r="O4" s="55"/>
+      <c r="P4" s="55"/>
+      <c r="Q4" s="55"/>
+      <c r="R4" s="55"/>
+      <c r="S4" s="55"/>
+      <c r="T4" s="55"/>
+      <c r="U4" s="56"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
@@ -2751,10 +2751,10 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="56"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -2778,10 +2778,10 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="56"/>
+      <c r="C7" s="57"/>
       <c r="D7" s="32"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -2826,44 +2826,44 @@
     </row>
     <row r="9" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="58"/>
-      <c r="E9" s="59" t="s">
+      <c r="D9" s="59"/>
+      <c r="E9" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="60" t="s">
+      <c r="F9" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="62" t="s">
+      <c r="G9" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="63"/>
-      <c r="L9" s="63"/>
-      <c r="M9" s="63"/>
-      <c r="N9" s="63"/>
-      <c r="O9" s="63"/>
-      <c r="P9" s="63"/>
-      <c r="Q9" s="63"/>
-      <c r="R9" s="63"/>
-      <c r="S9" s="63"/>
-      <c r="T9" s="63"/>
-      <c r="U9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="64"/>
+      <c r="K9" s="64"/>
+      <c r="L9" s="64"/>
+      <c r="M9" s="64"/>
+      <c r="N9" s="64"/>
+      <c r="O9" s="64"/>
+      <c r="P9" s="64"/>
+      <c r="Q9" s="64"/>
+      <c r="R9" s="64"/>
+      <c r="S9" s="64"/>
+      <c r="T9" s="64"/>
+      <c r="U9" s="65"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
-      <c r="B10" s="57"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="61"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="62"/>
       <c r="G10" s="23">
         <v>1</v>
       </c>
@@ -2912,12 +2912,12 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
-      <c r="B11" s="50">
+      <c r="B11" s="66">
         <v>1</v>
       </c>
-      <c r="C11" s="55"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="70"/>
       <c r="F11" s="25" t="s">
         <v>27</v>
       </c>
@@ -2939,10 +2939,10 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="54"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="71"/>
       <c r="F12" s="25" t="s">
         <v>28</v>
       </c>
@@ -2964,12 +2964,12 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
-      <c r="B13" s="50">
+      <c r="B13" s="66">
         <v>2</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="53"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="70"/>
       <c r="F13" s="25" t="s">
         <v>27</v>
       </c>
@@ -2991,10 +2991,10 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
-      <c r="B14" s="50"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="54"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="71"/>
       <c r="F14" s="25" t="s">
         <v>28</v>
       </c>
@@ -3016,12 +3016,12 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="20"/>
-      <c r="B15" s="50">
+      <c r="B15" s="66">
         <v>3</v>
       </c>
-      <c r="C15" s="55"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="53"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="70"/>
       <c r="F15" s="25" t="s">
         <v>27</v>
       </c>
@@ -3043,10 +3043,10 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
-      <c r="B16" s="50"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="54"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="71"/>
       <c r="F16" s="25" t="s">
         <v>28</v>
       </c>
@@ -3068,12 +3068,12 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
-      <c r="B17" s="50">
+      <c r="B17" s="66">
         <v>4</v>
       </c>
-      <c r="C17" s="55"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="53"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="70"/>
       <c r="F17" s="25" t="s">
         <v>27</v>
       </c>
@@ -3095,10 +3095,10 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
-      <c r="B18" s="50"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="54"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="71"/>
       <c r="F18" s="25" t="s">
         <v>28</v>
       </c>
@@ -3120,12 +3120,12 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="20"/>
-      <c r="B19" s="50">
+      <c r="B19" s="66">
         <v>5</v>
       </c>
-      <c r="C19" s="51"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="53"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="70"/>
       <c r="F19" s="25" t="s">
         <v>27</v>
       </c>
@@ -3147,10 +3147,10 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
-      <c r="B20" s="50"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="54"/>
+      <c r="B20" s="66"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="71"/>
       <c r="F20" s="25" t="s">
         <v>28</v>
       </c>
@@ -3172,12 +3172,12 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="20"/>
-      <c r="B21" s="50">
+      <c r="B21" s="66">
         <v>6</v>
       </c>
-      <c r="C21" s="55"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="53"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="70"/>
       <c r="F21" s="25" t="s">
         <v>27</v>
       </c>
@@ -3199,10 +3199,10 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="54"/>
+      <c r="B22" s="66"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="71"/>
       <c r="F22" s="25" t="s">
         <v>28</v>
       </c>
@@ -3224,12 +3224,12 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="20"/>
-      <c r="B23" s="50">
+      <c r="B23" s="66">
         <v>7</v>
       </c>
-      <c r="C23" s="51"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="53"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="70"/>
       <c r="F23" s="25" t="s">
         <v>27</v>
       </c>
@@ -3251,10 +3251,10 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="54"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="71"/>
       <c r="F24" s="25" t="s">
         <v>28</v>
       </c>
@@ -3276,12 +3276,12 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
-      <c r="B25" s="50">
+      <c r="B25" s="66">
         <v>8</v>
       </c>
-      <c r="C25" s="51"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="53"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="70"/>
       <c r="F25" s="25" t="s">
         <v>27</v>
       </c>
@@ -3303,10 +3303,10 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="54"/>
+      <c r="B26" s="66"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="71"/>
       <c r="F26" s="25" t="s">
         <v>28</v>
       </c>
@@ -3328,12 +3328,12 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
-      <c r="B27" s="50">
+      <c r="B27" s="66">
         <v>9</v>
       </c>
-      <c r="C27" s="51"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="53"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="70"/>
       <c r="F27" s="25" t="s">
         <v>27</v>
       </c>
@@ -3355,10 +3355,10 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
-      <c r="B28" s="50"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="54"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="71"/>
       <c r="F28" s="25" t="s">
         <v>28</v>
       </c>
@@ -3380,12 +3380,12 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
-      <c r="B29" s="50">
+      <c r="B29" s="66">
         <v>10</v>
       </c>
-      <c r="C29" s="51"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="53"/>
+      <c r="C29" s="69"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="70"/>
       <c r="F29" s="25" t="s">
         <v>27</v>
       </c>
@@ -3407,10 +3407,10 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
-      <c r="B30" s="50"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="54"/>
+      <c r="B30" s="66"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="68"/>
+      <c r="E30" s="71"/>
       <c r="F30" s="25" t="s">
         <v>28</v>
       </c>
@@ -3432,12 +3432,12 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="20"/>
-      <c r="B31" s="50">
+      <c r="B31" s="66">
         <v>11</v>
       </c>
-      <c r="C31" s="51"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="53"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="70"/>
       <c r="F31" s="25" t="s">
         <v>27</v>
       </c>
@@ -3459,10 +3459,10 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
-      <c r="B32" s="50"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="54"/>
+      <c r="B32" s="66"/>
+      <c r="C32" s="69"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="71"/>
       <c r="F32" s="25" t="s">
         <v>28</v>
       </c>
@@ -3484,12 +3484,12 @@
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="20"/>
-      <c r="B33" s="50">
+      <c r="B33" s="66">
         <v>12</v>
       </c>
-      <c r="C33" s="51"/>
-      <c r="D33" s="52"/>
-      <c r="E33" s="53"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="70"/>
       <c r="F33" s="25" t="s">
         <v>27</v>
       </c>
@@ -3511,10 +3511,10 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="15"/>
-      <c r="B34" s="50"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="52"/>
-      <c r="E34" s="54"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="71"/>
       <c r="F34" s="25" t="s">
         <v>28</v>
       </c>
@@ -3536,12 +3536,12 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="20"/>
-      <c r="B35" s="50">
+      <c r="B35" s="66">
         <v>13</v>
       </c>
-      <c r="C35" s="51"/>
-      <c r="D35" s="52"/>
-      <c r="E35" s="53"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="68"/>
+      <c r="E35" s="70"/>
       <c r="F35" s="25" t="s">
         <v>27</v>
       </c>
@@ -3563,10 +3563,10 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
-      <c r="B36" s="50"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="52"/>
-      <c r="E36" s="54"/>
+      <c r="B36" s="66"/>
+      <c r="C36" s="69"/>
+      <c r="D36" s="68"/>
+      <c r="E36" s="71"/>
       <c r="F36" s="25" t="s">
         <v>28</v>
       </c>
@@ -3588,12 +3588,12 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="20"/>
-      <c r="B37" s="50">
+      <c r="B37" s="66">
         <v>14</v>
       </c>
-      <c r="C37" s="51"/>
-      <c r="D37" s="52"/>
-      <c r="E37" s="53"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="68"/>
+      <c r="E37" s="70"/>
       <c r="F37" s="25" t="s">
         <v>27</v>
       </c>
@@ -3615,10 +3615,10 @@
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
-      <c r="B38" s="50"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="52"/>
-      <c r="E38" s="54"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="69"/>
+      <c r="D38" s="68"/>
+      <c r="E38" s="71"/>
       <c r="F38" s="25" t="s">
         <v>28</v>
       </c>
@@ -3640,12 +3640,12 @@
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="20"/>
-      <c r="B39" s="50">
+      <c r="B39" s="66">
         <v>15</v>
       </c>
-      <c r="C39" s="51"/>
-      <c r="D39" s="52"/>
-      <c r="E39" s="53"/>
+      <c r="C39" s="69"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="70"/>
       <c r="F39" s="25" t="s">
         <v>27</v>
       </c>
@@ -3667,10 +3667,10 @@
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
-      <c r="B40" s="50"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="52"/>
-      <c r="E40" s="54"/>
+      <c r="B40" s="66"/>
+      <c r="C40" s="69"/>
+      <c r="D40" s="68"/>
+      <c r="E40" s="71"/>
       <c r="F40" s="25" t="s">
         <v>28</v>
       </c>
@@ -3692,50 +3692,6 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B2:U4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:U9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:D34"/>
-    <mergeCell ref="E33:E34"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="C39:D40"/>
     <mergeCell ref="E39:E40"/>
@@ -3745,6 +3701,50 @@
     <mergeCell ref="B37:B38"/>
     <mergeCell ref="C37:D38"/>
     <mergeCell ref="E37:E38"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="B2:U4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:U9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
jdre-16/03/2015-Se modifico BITACORA.xlsx, se renombro el archivo MI_11032015_RETROALIMENTACION.docx
</commit_message>
<xml_diff>
--- a/ afgmx/AFGMX/ADMON_DEL_PROYECTO/BITACORAS/2015/CUAT_1_ENER_ABR/PARCIAL_3/BITACORA.xlsx
+++ b/ afgmx/AFGMX/ADMON_DEL_PROYECTO/BITACORAS/2015/CUAT_1_ENER_ABR/PARCIAL_3/BITACORA.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
   <si>
     <t>UNIVERSIDAD TECNOLÓGICA DEL  CENTRO DE VERACRUZ
 TECNOLOGÍAS DE LA INFORMACIÓN Y COMUNICACIÓN
@@ -197,16 +197,31 @@
     <t>Finalizado</t>
   </si>
   <si>
-    <t>Se realizo el registro del proyecto en www.posible.org que se anexa como REGISTRO_POSIBLE y se levanto una minuta que se anexa con el nombre de MINUTA</t>
-  </si>
-  <si>
-    <t>Bitácora, minuta y comprobante de inscripción en posible.org</t>
-  </si>
-  <si>
-    <t>Juan Diego Romero Espinoza, Carlos Enrique Hernandez Jiménez e Ing. Ramiro Alcazar Magaña</t>
-  </si>
-  <si>
     <t>Incripción a posible y acuerdos para el desarrollo del software</t>
+  </si>
+  <si>
+    <t>Retroalimentacion por parte del asesor academico Ing. Ramiro Alcazar Magaña</t>
+  </si>
+  <si>
+    <t>Se realizo el registro del proyecto en www.posible.org que se anexa como REGISTRO_POSIBLE</t>
+  </si>
+  <si>
+    <t>Se levanto una minuta y se anexa como MI_11032015_RETROALIMENTACION</t>
+  </si>
+  <si>
+    <t>Minuta</t>
+  </si>
+  <si>
+    <t>Bitácora y comprobante de inscripción en posible.org</t>
+  </si>
+  <si>
+    <t>Carlos Enrique Hernandez Jiménez e Ing. Ramiro Alcazar Magaña</t>
+  </si>
+  <si>
+    <t>Juan Diego Romero Espinoza</t>
+  </si>
+  <si>
+    <t>AgroFinderGround</t>
   </si>
 </sst>
 </file>
@@ -217,7 +232,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="d/m/yy;@"/>
   </numFmts>
-  <fonts count="55" x14ac:knownFonts="1">
+  <fonts count="56" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -512,6 +527,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1228,7 +1250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1292,7 +1314,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="54" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1305,6 +1326,27 @@
     <xf numFmtId="0" fontId="53" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="22" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1323,27 +1365,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="22" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1353,6 +1374,24 @@
     <xf numFmtId="0" fontId="53" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1389,22 +1428,14 @@
     <xf numFmtId="0" fontId="12" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="53" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="54" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1896,7 +1927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1926,46 +1957,46 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="40"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="46"/>
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="40"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="46"/>
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="40"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="46"/>
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1988,13 +2019,13 @@
       <c r="C6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
@@ -2006,13 +2037,13 @@
       <c r="C7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
@@ -2024,13 +2055,13 @@
       <c r="C8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="43" t="s">
+      <c r="D8" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -2042,13 +2073,13 @@
       <c r="C9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
       <c r="I9" s="15"/>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
@@ -2060,13 +2091,13 @@
       <c r="C10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="44">
+      <c r="D10" s="39">
         <v>1</v>
       </c>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
@@ -2078,13 +2109,13 @@
       <c r="C11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="47" t="s">
+      <c r="D11" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
@@ -2110,11 +2141,11 @@
       <c r="C13" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
       <c r="I13" s="15"/>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
@@ -2126,13 +2157,13 @@
       <c r="C14" s="26">
         <v>1</v>
       </c>
-      <c r="D14" s="49" t="s">
+      <c r="D14" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
@@ -2144,13 +2175,13 @@
       <c r="C15" s="26">
         <v>2</v>
       </c>
-      <c r="D15" s="45" t="s">
+      <c r="D15" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
@@ -2162,13 +2193,13 @@
       <c r="C16" s="26">
         <v>3</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="D16" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
       <c r="I16" s="15"/>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
@@ -2180,13 +2211,13 @@
       <c r="C17" s="26">
         <v>4</v>
       </c>
-      <c r="D17" s="45" t="s">
+      <c r="D17" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
@@ -2198,13 +2229,13 @@
       <c r="C18" s="26">
         <v>5</v>
       </c>
-      <c r="D18" s="45" t="s">
+      <c r="D18" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
@@ -2216,11 +2247,11 @@
       <c r="C19" s="26">
         <v>6</v>
       </c>
-      <c r="D19" s="45"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
@@ -2242,6 +2273,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B2:K4"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="D9:H9"/>
     <mergeCell ref="D16:H16"/>
     <mergeCell ref="D17:H17"/>
     <mergeCell ref="D18:H18"/>
@@ -2251,11 +2287,6 @@
     <mergeCell ref="D13:H13"/>
     <mergeCell ref="D14:H14"/>
     <mergeCell ref="D15:H15"/>
-    <mergeCell ref="B2:K4"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="D9:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2266,8 +2297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2311,42 +2342,42 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="53"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="52"/>
       <c r="J3" s="19"/>
       <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
-      <c r="B4" s="51"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="53"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="52"/>
       <c r="J4" s="19"/>
       <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
-      <c r="B5" s="51"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="53"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="52"/>
       <c r="J5" s="19"/>
       <c r="K5" s="7"/>
     </row>
@@ -2407,40 +2438,54 @@
     </row>
     <row r="9" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
-      <c r="B9" s="35">
-        <v>1</v>
-      </c>
-      <c r="C9" s="36">
+      <c r="B9" s="34">
+        <v>10</v>
+      </c>
+      <c r="C9" s="35">
         <v>42074</v>
       </c>
-      <c r="D9" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="35" t="s">
+      <c r="D9" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="34" t="s">
         <v>54</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="I9" s="37"/>
+        <v>61</v>
+      </c>
+      <c r="I9" s="36"/>
       <c r="J9" s="2"/>
       <c r="K9" s="15"/>
     </row>
     <row r="10" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="22"/>
+      <c r="B10" s="34">
+        <v>10</v>
+      </c>
+      <c r="C10" s="71">
+        <v>42311</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="72" t="s">
+        <v>62</v>
+      </c>
       <c r="I10" s="13"/>
       <c r="J10" s="2"/>
       <c r="K10" s="15"/>
@@ -2618,8 +2663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:D28"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2657,74 +2702,74 @@
     </row>
     <row r="2" spans="1:21" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="56"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="60"/>
+      <c r="U2" s="61"/>
     </row>
     <row r="3" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="55"/>
-      <c r="S3" s="55"/>
-      <c r="T3" s="55"/>
-      <c r="U3" s="56"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60"/>
+      <c r="R3" s="60"/>
+      <c r="S3" s="60"/>
+      <c r="T3" s="60"/>
+      <c r="U3" s="61"/>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
-      <c r="M4" s="55"/>
-      <c r="N4" s="55"/>
-      <c r="O4" s="55"/>
-      <c r="P4" s="55"/>
-      <c r="Q4" s="55"/>
-      <c r="R4" s="55"/>
-      <c r="S4" s="55"/>
-      <c r="T4" s="55"/>
-      <c r="U4" s="56"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
+      <c r="P4" s="60"/>
+      <c r="Q4" s="60"/>
+      <c r="R4" s="60"/>
+      <c r="S4" s="60"/>
+      <c r="T4" s="60"/>
+      <c r="U4" s="61"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
@@ -2751,11 +2796,13 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="1"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="73" t="s">
+        <v>63</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="15"/>
@@ -2769,19 +2816,21 @@
       <c r="M6" s="15"/>
       <c r="N6" s="15"/>
       <c r="O6" s="15"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
+      <c r="P6" s="74">
+        <v>42074</v>
+      </c>
+      <c r="Q6" s="74"/>
+      <c r="R6" s="74"/>
+      <c r="S6" s="74"/>
+      <c r="T6" s="74"/>
+      <c r="U6" s="74"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="57"/>
+      <c r="C7" s="62"/>
       <c r="D7" s="32"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -2826,44 +2875,44 @@
     </row>
     <row r="9" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="59"/>
-      <c r="E9" s="60" t="s">
+      <c r="D9" s="64"/>
+      <c r="E9" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="61" t="s">
+      <c r="F9" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="63" t="s">
+      <c r="G9" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="64"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="64"/>
-      <c r="K9" s="64"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="64"/>
-      <c r="N9" s="64"/>
-      <c r="O9" s="64"/>
-      <c r="P9" s="64"/>
-      <c r="Q9" s="64"/>
-      <c r="R9" s="64"/>
-      <c r="S9" s="64"/>
-      <c r="T9" s="64"/>
-      <c r="U9" s="65"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="69"/>
+      <c r="M9" s="69"/>
+      <c r="N9" s="69"/>
+      <c r="O9" s="69"/>
+      <c r="P9" s="69"/>
+      <c r="Q9" s="69"/>
+      <c r="R9" s="69"/>
+      <c r="S9" s="69"/>
+      <c r="T9" s="69"/>
+      <c r="U9" s="70"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
-      <c r="B10" s="58"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="62"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="67"/>
       <c r="G10" s="23">
         <v>1</v>
       </c>
@@ -2912,12 +2961,12 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
-      <c r="B11" s="66">
+      <c r="B11" s="53">
         <v>1</v>
       </c>
-      <c r="C11" s="67"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="70"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="56"/>
       <c r="F11" s="25" t="s">
         <v>27</v>
       </c>
@@ -2939,10 +2988,10 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
-      <c r="B12" s="66"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="71"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="57"/>
       <c r="F12" s="25" t="s">
         <v>28</v>
       </c>
@@ -2964,12 +3013,12 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
-      <c r="B13" s="66">
+      <c r="B13" s="53">
         <v>2</v>
       </c>
-      <c r="C13" s="69"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="70"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="56"/>
       <c r="F13" s="25" t="s">
         <v>27</v>
       </c>
@@ -2991,10 +3040,10 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="69"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="71"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="57"/>
       <c r="F14" s="25" t="s">
         <v>28</v>
       </c>
@@ -3016,12 +3065,12 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="20"/>
-      <c r="B15" s="66">
+      <c r="B15" s="53">
         <v>3</v>
       </c>
-      <c r="C15" s="67"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="70"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="56"/>
       <c r="F15" s="25" t="s">
         <v>27</v>
       </c>
@@ -3043,10 +3092,10 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="71"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="57"/>
       <c r="F16" s="25" t="s">
         <v>28</v>
       </c>
@@ -3068,12 +3117,12 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
-      <c r="B17" s="66">
+      <c r="B17" s="53">
         <v>4</v>
       </c>
-      <c r="C17" s="67"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="70"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="56"/>
       <c r="F17" s="25" t="s">
         <v>27</v>
       </c>
@@ -3095,10 +3144,10 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
-      <c r="B18" s="66"/>
-      <c r="C18" s="69"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="71"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="57"/>
       <c r="F18" s="25" t="s">
         <v>28</v>
       </c>
@@ -3120,12 +3169,12 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="20"/>
-      <c r="B19" s="66">
+      <c r="B19" s="53">
         <v>5</v>
       </c>
-      <c r="C19" s="69"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="70"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="56"/>
       <c r="F19" s="25" t="s">
         <v>27</v>
       </c>
@@ -3147,10 +3196,10 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
-      <c r="B20" s="66"/>
-      <c r="C20" s="69"/>
-      <c r="D20" s="68"/>
-      <c r="E20" s="71"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="57"/>
       <c r="F20" s="25" t="s">
         <v>28</v>
       </c>
@@ -3172,12 +3221,12 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="20"/>
-      <c r="B21" s="66">
+      <c r="B21" s="53">
         <v>6</v>
       </c>
-      <c r="C21" s="67"/>
-      <c r="D21" s="68"/>
-      <c r="E21" s="70"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="56"/>
       <c r="F21" s="25" t="s">
         <v>27</v>
       </c>
@@ -3199,10 +3248,10 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
-      <c r="B22" s="66"/>
-      <c r="C22" s="69"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="71"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="57"/>
       <c r="F22" s="25" t="s">
         <v>28</v>
       </c>
@@ -3224,12 +3273,12 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="20"/>
-      <c r="B23" s="66">
+      <c r="B23" s="53">
         <v>7</v>
       </c>
-      <c r="C23" s="69"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="70"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="56"/>
       <c r="F23" s="25" t="s">
         <v>27</v>
       </c>
@@ -3251,10 +3300,10 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
-      <c r="B24" s="66"/>
-      <c r="C24" s="69"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="71"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="57"/>
       <c r="F24" s="25" t="s">
         <v>28</v>
       </c>
@@ -3276,12 +3325,12 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
-      <c r="B25" s="66">
+      <c r="B25" s="53">
         <v>8</v>
       </c>
-      <c r="C25" s="69"/>
-      <c r="D25" s="68"/>
-      <c r="E25" s="70"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="56"/>
       <c r="F25" s="25" t="s">
         <v>27</v>
       </c>
@@ -3303,10 +3352,10 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
-      <c r="B26" s="66"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="68"/>
-      <c r="E26" s="71"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="57"/>
       <c r="F26" s="25" t="s">
         <v>28</v>
       </c>
@@ -3328,12 +3377,12 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
-      <c r="B27" s="66">
+      <c r="B27" s="53">
         <v>9</v>
       </c>
-      <c r="C27" s="69"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="70"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="56"/>
       <c r="F27" s="25" t="s">
         <v>27</v>
       </c>
@@ -3355,10 +3404,10 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
-      <c r="B28" s="66"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="71"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="57"/>
       <c r="F28" s="25" t="s">
         <v>28</v>
       </c>
@@ -3380,12 +3429,12 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
-      <c r="B29" s="66">
+      <c r="B29" s="53">
         <v>10</v>
       </c>
-      <c r="C29" s="69"/>
-      <c r="D29" s="68"/>
-      <c r="E29" s="70"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="56"/>
       <c r="F29" s="25" t="s">
         <v>27</v>
       </c>
@@ -3407,10 +3456,10 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
-      <c r="B30" s="66"/>
-      <c r="C30" s="69"/>
-      <c r="D30" s="68"/>
-      <c r="E30" s="71"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="57"/>
       <c r="F30" s="25" t="s">
         <v>28</v>
       </c>
@@ -3432,12 +3481,12 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="20"/>
-      <c r="B31" s="66">
+      <c r="B31" s="53">
         <v>11</v>
       </c>
-      <c r="C31" s="69"/>
-      <c r="D31" s="68"/>
-      <c r="E31" s="70"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="56"/>
       <c r="F31" s="25" t="s">
         <v>27</v>
       </c>
@@ -3459,10 +3508,10 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
-      <c r="B32" s="66"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="68"/>
-      <c r="E32" s="71"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="57"/>
       <c r="F32" s="25" t="s">
         <v>28</v>
       </c>
@@ -3484,12 +3533,12 @@
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="20"/>
-      <c r="B33" s="66">
+      <c r="B33" s="53">
         <v>12</v>
       </c>
-      <c r="C33" s="69"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="70"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="56"/>
       <c r="F33" s="25" t="s">
         <v>27</v>
       </c>
@@ -3511,10 +3560,10 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="15"/>
-      <c r="B34" s="66"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="71"/>
+      <c r="B34" s="53"/>
+      <c r="C34" s="54"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="57"/>
       <c r="F34" s="25" t="s">
         <v>28</v>
       </c>
@@ -3536,12 +3585,12 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="20"/>
-      <c r="B35" s="66">
+      <c r="B35" s="53">
         <v>13</v>
       </c>
-      <c r="C35" s="69"/>
-      <c r="D35" s="68"/>
-      <c r="E35" s="70"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="56"/>
       <c r="F35" s="25" t="s">
         <v>27</v>
       </c>
@@ -3563,10 +3612,10 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
-      <c r="B36" s="66"/>
-      <c r="C36" s="69"/>
-      <c r="D36" s="68"/>
-      <c r="E36" s="71"/>
+      <c r="B36" s="53"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="57"/>
       <c r="F36" s="25" t="s">
         <v>28</v>
       </c>
@@ -3588,12 +3637,12 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="20"/>
-      <c r="B37" s="66">
+      <c r="B37" s="53">
         <v>14</v>
       </c>
-      <c r="C37" s="69"/>
-      <c r="D37" s="68"/>
-      <c r="E37" s="70"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="56"/>
       <c r="F37" s="25" t="s">
         <v>27</v>
       </c>
@@ -3615,10 +3664,10 @@
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
-      <c r="B38" s="66"/>
-      <c r="C38" s="69"/>
-      <c r="D38" s="68"/>
-      <c r="E38" s="71"/>
+      <c r="B38" s="53"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="57"/>
       <c r="F38" s="25" t="s">
         <v>28</v>
       </c>
@@ -3640,12 +3689,12 @@
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="20"/>
-      <c r="B39" s="66">
+      <c r="B39" s="53">
         <v>15</v>
       </c>
-      <c r="C39" s="69"/>
-      <c r="D39" s="68"/>
-      <c r="E39" s="70"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="56"/>
       <c r="F39" s="25" t="s">
         <v>27</v>
       </c>
@@ -3667,10 +3716,10 @@
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
-      <c r="B40" s="66"/>
-      <c r="C40" s="69"/>
-      <c r="D40" s="68"/>
-      <c r="E40" s="71"/>
+      <c r="B40" s="53"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="57"/>
       <c r="F40" s="25" t="s">
         <v>28</v>
       </c>
@@ -3691,7 +3740,52 @@
       <c r="U40" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="53">
+  <mergeCells count="54">
+    <mergeCell ref="B2:U4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:U9"/>
+    <mergeCell ref="P6:U6"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:D34"/>
+    <mergeCell ref="E33:E34"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="C39:D40"/>
     <mergeCell ref="E39:E40"/>
@@ -3701,50 +3795,6 @@
     <mergeCell ref="B37:B38"/>
     <mergeCell ref="C37:D38"/>
     <mergeCell ref="E37:E38"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="B2:U4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:U9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
jdre-18/03/2015-Se actualiza la BITACORA.xlsx con la reunion de hoy anexando la MI_18032015_REVISION_Y_ASIGNACION_DE_TAREAS.docx como respaldo de los acuerdos tomados y se actualizo el documento ARQ_DE_SW.docx que se le incluyo la vista de despliegue
</commit_message>
<xml_diff>
--- a/ afgmx/AFGMX/ADMON_DEL_PROYECTO/BITACORAS/2015/CUAT_1_ENER_ABR/PARCIAL_3/BITACORA.xlsx
+++ b/ afgmx/AFGMX/ADMON_DEL_PROYECTO/BITACORAS/2015/CUAT_1_ENER_ABR/PARCIAL_3/BITACORA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="19440" windowHeight="8340" activeTab="1"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="19440" windowHeight="8340" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="77">
   <si>
     <t>UNIVERSIDAD TECNOLÓGICA DEL  CENTRO DE VERACRUZ
 TECNOLOGÍAS DE LA INFORMACIÓN Y COMUNICACIÓN
@@ -222,6 +222,45 @@
   </si>
   <si>
     <t>AgroFinderGround</t>
+  </si>
+  <si>
+    <t>Asignacion de investigacion sobre software de tercero Diarihuana</t>
+  </si>
+  <si>
+    <t>Se levanto una minuta donde se acordo quien estaria encargado de dicha actividad</t>
+  </si>
+  <si>
+    <t>Asignacion de investigacion sobre software de tercero Haifa Nutri-Net</t>
+  </si>
+  <si>
+    <t>Carlos Enrique Hernandez Jiménez</t>
+  </si>
+  <si>
+    <t>Revision de avance con respecto a la aplicación</t>
+  </si>
+  <si>
+    <t>Se evaluo el avance actual con la comparacion de la anterior sesion</t>
+  </si>
+  <si>
+    <t>Ramiro Alcazar Magaña</t>
+  </si>
+  <si>
+    <t>Acuerdo para nuevas actividades, con respecto para esta semana como son las investigaciones, documentación, etc.</t>
+  </si>
+  <si>
+    <t>Se levanto una minuta que se anexa como MI_18032015_REVISION_Y_ASIGNACION_DE_TAREAS</t>
+  </si>
+  <si>
+    <t>Leonardo Luna Ruiz</t>
+  </si>
+  <si>
+    <t>Actualizacion de bitacora</t>
+  </si>
+  <si>
+    <t>Se actulizo la bitacora con las actividades de la semana 11 que corresponde al parcial 3</t>
+  </si>
+  <si>
+    <t>Biacora</t>
   </si>
 </sst>
 </file>
@@ -232,7 +271,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="d/m/yy;@"/>
   </numFmts>
-  <fonts count="56" x14ac:knownFonts="1">
+  <fonts count="54" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -360,12 +399,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
     </font>
     <font>
       <b/>
@@ -527,13 +560,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1250,7 +1276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1270,75 +1296,88 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="19" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="20" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="17" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="19" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="47" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="48" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="53" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="52" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="53" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="22" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="22" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1347,96 +1386,86 @@
     <xf numFmtId="0" fontId="23" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="24" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="18" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="53" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="52" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="24" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="18" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="53" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="54" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1942,65 +1971,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="15"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="14"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="46"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="38"/>
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="46"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="38"/>
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="46"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="38"/>
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -2011,273 +2040,268 @@
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
-      <c r="L5" s="15"/>
+      <c r="L5" s="14"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
       <c r="C6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="49" t="s">
+      <c r="D7" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="49" t="s">
+      <c r="D8" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="39">
+      <c r="D10" s="42">
         <v>1</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D11" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="12" t="s">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="26">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="25">
         <v>1</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="26">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="25">
         <v>2</v>
       </c>
-      <c r="D15" s="37" t="s">
+      <c r="D15" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="26">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="25">
         <v>3</v>
       </c>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="26">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="25">
         <v>4</v>
       </c>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="26">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="25">
         <v>5</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="D18" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="26">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="25">
         <v>6</v>
       </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B2:K4"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="D9:H9"/>
     <mergeCell ref="D16:H16"/>
     <mergeCell ref="D17:H17"/>
     <mergeCell ref="D18:H18"/>
@@ -2287,6 +2311,11 @@
     <mergeCell ref="D13:H13"/>
     <mergeCell ref="D14:H14"/>
     <mergeCell ref="D15:H15"/>
+    <mergeCell ref="B2:K4"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="D9:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2297,8 +2326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2308,81 +2337,81 @@
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
     <col min="4" max="4" width="76.28515625" customWidth="1"/>
     <col min="5" max="5" width="24.5703125" customWidth="1"/>
-    <col min="6" max="6" width="159" customWidth="1"/>
-    <col min="7" max="7" width="78.85546875" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="112.85546875" customWidth="1"/>
+    <col min="7" max="7" width="64.140625" customWidth="1"/>
+    <col min="8" max="8" width="73" customWidth="1"/>
     <col min="9" max="9" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="19"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="18"/>
       <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="19"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="18"/>
       <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="19"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="18"/>
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -2391,11 +2420,11 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -2404,244 +2433,314 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="20" t="s">
         <v>16</v>
       </c>
       <c r="J8" s="2"/>
-      <c r="K8" s="15"/>
+      <c r="K8" s="14"/>
     </row>
     <row r="9" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="34">
+      <c r="A9" s="19"/>
+      <c r="B9" s="32">
         <v>10</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="71">
         <v>42074</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="28" t="s">
+      <c r="H9" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="I9" s="36"/>
+      <c r="I9" s="33"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="15"/>
+      <c r="K9" s="14"/>
     </row>
     <row r="10" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="34">
+      <c r="A10" s="19"/>
+      <c r="B10" s="32">
         <v>10</v>
       </c>
-      <c r="C10" s="71">
-        <v>42311</v>
-      </c>
-      <c r="D10" s="28" t="s">
+      <c r="C10" s="34">
+        <v>42074</v>
+      </c>
+      <c r="D10" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E10" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="H10" s="72" t="s">
+      <c r="H10" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="I10" s="13"/>
+      <c r="I10" s="12"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="15"/>
+      <c r="K10" s="14"/>
     </row>
     <row r="11" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="13"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="32">
+        <v>11</v>
+      </c>
+      <c r="C11" s="34">
+        <v>42081</v>
+      </c>
+      <c r="D11" s="73" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="12"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="15"/>
+      <c r="K11" s="14"/>
     </row>
     <row r="12" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="13"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="32">
+        <v>11</v>
+      </c>
+      <c r="C12" s="34">
+        <v>42081</v>
+      </c>
+      <c r="D12" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="72"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="15"/>
+      <c r="K12" s="14"/>
     </row>
     <row r="13" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="13"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="32">
+        <v>11</v>
+      </c>
+      <c r="C13" s="34">
+        <v>42081</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="I13" s="72"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="15"/>
+      <c r="K13" s="14"/>
     </row>
     <row r="14" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="13"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="32">
+        <v>11</v>
+      </c>
+      <c r="C14" s="34">
+        <v>42081</v>
+      </c>
+      <c r="D14" s="75" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" s="72"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="15"/>
+      <c r="K14" s="14"/>
     </row>
     <row r="15" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="13"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="32">
+        <v>11</v>
+      </c>
+      <c r="C15" s="34">
+        <v>42081</v>
+      </c>
+      <c r="D15" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="72"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="15"/>
+      <c r="K15" s="14"/>
     </row>
     <row r="16" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="13"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="12"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="15"/>
+      <c r="K16" s="14"/>
     </row>
     <row r="17" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="13"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="12"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="15"/>
+      <c r="K17" s="14"/>
     </row>
     <row r="18" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="13"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="12"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="15"/>
+      <c r="K18" s="14"/>
     </row>
     <row r="19" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="13"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="12"/>
       <c r="J19" s="2"/>
-      <c r="K19" s="15"/>
+      <c r="K19" s="14"/>
     </row>
     <row r="20" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="13"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="12"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="15"/>
+      <c r="K20" s="14"/>
     </row>
     <row r="21" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="13"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="12"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="15"/>
+      <c r="K21" s="14"/>
     </row>
     <row r="22" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
+      <c r="A22" s="19"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="15"/>
+      <c r="K22" s="14"/>
     </row>
     <row r="23" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
+      <c r="A23" s="19"/>
       <c r="J23" s="2"/>
-      <c r="K23" s="15"/>
+      <c r="K23" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2663,7 +2762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
@@ -2678,101 +2777,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
     </row>
     <row r="2" spans="1:21" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="60"/>
-      <c r="R2" s="60"/>
-      <c r="S2" s="60"/>
-      <c r="T2" s="60"/>
-      <c r="U2" s="61"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="54"/>
     </row>
     <row r="3" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="60"/>
-      <c r="R3" s="60"/>
-      <c r="S3" s="60"/>
-      <c r="T3" s="60"/>
-      <c r="U3" s="61"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="53"/>
+      <c r="Q3" s="53"/>
+      <c r="R3" s="53"/>
+      <c r="S3" s="53"/>
+      <c r="T3" s="53"/>
+      <c r="U3" s="54"/>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="60"/>
-      <c r="P4" s="60"/>
-      <c r="Q4" s="60"/>
-      <c r="R4" s="60"/>
-      <c r="S4" s="60"/>
-      <c r="T4" s="60"/>
-      <c r="U4" s="61"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="53"/>
+      <c r="M4" s="53"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="53"/>
+      <c r="P4" s="53"/>
+      <c r="Q4" s="53"/>
+      <c r="R4" s="53"/>
+      <c r="S4" s="53"/>
+      <c r="T4" s="53"/>
+      <c r="U4" s="54"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -2795,63 +2894,63 @@
       <c r="U5" s="6"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="62" t="s">
+      <c r="A6" s="14"/>
+      <c r="B6" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="62"/>
-      <c r="D6" s="73" t="s">
+      <c r="C6" s="55"/>
+      <c r="D6" s="35" t="s">
         <v>63</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="18" t="s">
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="74">
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="64">
         <v>42074</v>
       </c>
-      <c r="Q6" s="74"/>
-      <c r="R6" s="74"/>
-      <c r="S6" s="74"/>
-      <c r="T6" s="74"/>
-      <c r="U6" s="74"/>
+      <c r="Q6" s="64"/>
+      <c r="R6" s="64"/>
+      <c r="S6" s="64"/>
+      <c r="T6" s="64"/>
+      <c r="U6" s="64"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="62" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="62"/>
-      <c r="D7" s="32"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="30"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="27"/>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27"/>
-      <c r="U7" s="27"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="26"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="5"/>
@@ -2874,873 +2973,918 @@
       <c r="U8" s="1"/>
     </row>
     <row r="9" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="63" t="s">
+      <c r="A9" s="19"/>
+      <c r="B9" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="64" t="s">
+      <c r="C9" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="64"/>
-      <c r="E9" s="65" t="s">
+      <c r="D9" s="57"/>
+      <c r="E9" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="66" t="s">
+      <c r="F9" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="68" t="s">
+      <c r="G9" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="69"/>
-      <c r="K9" s="69"/>
-      <c r="L9" s="69"/>
-      <c r="M9" s="69"/>
-      <c r="N9" s="69"/>
-      <c r="O9" s="69"/>
-      <c r="P9" s="69"/>
-      <c r="Q9" s="69"/>
-      <c r="R9" s="69"/>
-      <c r="S9" s="69"/>
-      <c r="T9" s="69"/>
-      <c r="U9" s="70"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="62"/>
+      <c r="K9" s="62"/>
+      <c r="L9" s="62"/>
+      <c r="M9" s="62"/>
+      <c r="N9" s="62"/>
+      <c r="O9" s="62"/>
+      <c r="P9" s="62"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="62"/>
+      <c r="S9" s="62"/>
+      <c r="T9" s="62"/>
+      <c r="U9" s="63"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="23">
+      <c r="A10" s="14"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="22">
         <v>1</v>
       </c>
-      <c r="H10" s="23">
+      <c r="H10" s="22">
         <v>2</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="22">
         <v>3</v>
       </c>
-      <c r="J10" s="23">
+      <c r="J10" s="22">
         <v>4</v>
       </c>
-      <c r="K10" s="23">
+      <c r="K10" s="22">
         <v>5</v>
       </c>
-      <c r="L10" s="23">
+      <c r="L10" s="22">
         <v>6</v>
       </c>
-      <c r="M10" s="23">
+      <c r="M10" s="22">
         <v>7</v>
       </c>
-      <c r="N10" s="23">
+      <c r="N10" s="22">
         <v>8</v>
       </c>
-      <c r="O10" s="23">
+      <c r="O10" s="22">
         <v>9</v>
       </c>
-      <c r="P10" s="23">
+      <c r="P10" s="22">
         <v>10</v>
       </c>
-      <c r="Q10" s="23">
+      <c r="Q10" s="22">
         <v>11</v>
       </c>
-      <c r="R10" s="23">
+      <c r="R10" s="22">
         <v>12</v>
       </c>
-      <c r="S10" s="23">
+      <c r="S10" s="22">
         <v>13</v>
       </c>
-      <c r="T10" s="23">
+      <c r="T10" s="22">
         <v>14</v>
       </c>
-      <c r="U10" s="23">
+      <c r="U10" s="22">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="53">
+      <c r="A11" s="19"/>
+      <c r="B11" s="65">
         <v>1</v>
       </c>
-      <c r="C11" s="58"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="25" t="s">
+      <c r="C11" s="66"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
-      <c r="T11" s="25"/>
-      <c r="U11" s="25"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="24"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="25" t="s">
+      <c r="A12" s="14"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
-      <c r="T12" s="25"/>
-      <c r="U12" s="25"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="24"/>
+      <c r="T12" s="24"/>
+      <c r="U12" s="24"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="53">
+      <c r="A13" s="19"/>
+      <c r="B13" s="65">
         <v>2</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="25" t="s">
+      <c r="C13" s="68"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="24" t="s">
         <v>27</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="25"/>
-      <c r="T13" s="25"/>
-      <c r="U13" s="25"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="24"/>
+      <c r="S13" s="24"/>
+      <c r="T13" s="24"/>
+      <c r="U13" s="24"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="53"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="25" t="s">
+      <c r="A14" s="14"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="25"/>
-      <c r="T14" s="25"/>
-      <c r="U14" s="25"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="24"/>
+      <c r="U14" s="24"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="53">
+      <c r="A15" s="19"/>
+      <c r="B15" s="65">
         <v>3</v>
       </c>
-      <c r="C15" s="58"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="25" t="s">
+      <c r="C15" s="66"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="25"/>
-      <c r="T15" s="25"/>
-      <c r="U15" s="25"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
+      <c r="T15" s="24"/>
+      <c r="U15" s="24"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="53"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="25" t="s">
+      <c r="A16" s="14"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="25"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="25"/>
-      <c r="T16" s="25"/>
-      <c r="U16" s="25"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="24"/>
+      <c r="T16" s="24"/>
+      <c r="U16" s="24"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="53">
+      <c r="A17" s="19"/>
+      <c r="B17" s="65">
         <v>4</v>
       </c>
-      <c r="C17" s="58"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="25" t="s">
+      <c r="C17" s="66"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
       <c r="J17" s="10"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="25"/>
-      <c r="S17" s="25"/>
-      <c r="T17" s="25"/>
-      <c r="U17" s="25"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="24"/>
+      <c r="S17" s="24"/>
+      <c r="T17" s="24"/>
+      <c r="U17" s="24"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="25" t="s">
+      <c r="A18" s="14"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25"/>
-      <c r="P18" s="25"/>
-      <c r="Q18" s="25"/>
-      <c r="R18" s="25"/>
-      <c r="S18" s="25"/>
-      <c r="T18" s="25"/>
-      <c r="U18" s="25"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
+      <c r="S18" s="24"/>
+      <c r="T18" s="24"/>
+      <c r="U18" s="24"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="53">
+      <c r="A19" s="19"/>
+      <c r="B19" s="65">
         <v>5</v>
       </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="25" t="s">
+      <c r="C19" s="68"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="25"/>
-      <c r="O19" s="25"/>
-      <c r="P19" s="25"/>
-      <c r="Q19" s="25"/>
-      <c r="R19" s="25"/>
-      <c r="S19" s="25"/>
-      <c r="T19" s="25"/>
-      <c r="U19" s="25"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="24"/>
+      <c r="S19" s="24"/>
+      <c r="T19" s="24"/>
+      <c r="U19" s="24"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="25" t="s">
+      <c r="A20" s="14"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="68"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="25"/>
-      <c r="O20" s="25"/>
-      <c r="P20" s="25"/>
-      <c r="Q20" s="25"/>
-      <c r="R20" s="25"/>
-      <c r="S20" s="25"/>
-      <c r="T20" s="25"/>
-      <c r="U20" s="25"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="24"/>
+      <c r="U20" s="24"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="53">
+      <c r="A21" s="19"/>
+      <c r="B21" s="65">
         <v>6</v>
       </c>
-      <c r="C21" s="58"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="25" t="s">
+      <c r="C21" s="66"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
       <c r="P21" s="10"/>
-      <c r="Q21" s="25"/>
-      <c r="R21" s="25"/>
-      <c r="S21" s="25"/>
-      <c r="T21" s="25"/>
-      <c r="U21" s="25"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="24"/>
+      <c r="S21" s="24"/>
+      <c r="T21" s="24"/>
+      <c r="U21" s="24"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="54"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="25" t="s">
+      <c r="A22" s="14"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="25"/>
-      <c r="O22" s="25"/>
-      <c r="P22" s="25"/>
-      <c r="Q22" s="25"/>
-      <c r="R22" s="25"/>
-      <c r="S22" s="25"/>
-      <c r="T22" s="25"/>
-      <c r="U22" s="25"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="24"/>
+      <c r="S22" s="24"/>
+      <c r="T22" s="24"/>
+      <c r="U22" s="24"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
-      <c r="B23" s="53">
+      <c r="A23" s="19"/>
+      <c r="B23" s="65">
         <v>7</v>
       </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="25" t="s">
+      <c r="C23" s="68"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="25"/>
-      <c r="P23" s="25"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="24"/>
       <c r="Q23" s="10"/>
       <c r="R23" s="10"/>
-      <c r="S23" s="25"/>
-      <c r="T23" s="25"/>
-      <c r="U23" s="25"/>
+      <c r="S23" s="24"/>
+      <c r="T23" s="24"/>
+      <c r="U23" s="24"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="25" t="s">
+      <c r="A24" s="14"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="25"/>
-      <c r="O24" s="25"/>
-      <c r="P24" s="25"/>
-      <c r="Q24" s="25"/>
-      <c r="R24" s="25"/>
-      <c r="S24" s="25"/>
-      <c r="T24" s="25"/>
-      <c r="U24" s="25"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="24"/>
+      <c r="R24" s="24"/>
+      <c r="S24" s="24"/>
+      <c r="T24" s="24"/>
+      <c r="U24" s="24"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
-      <c r="B25" s="53">
+      <c r="A25" s="19"/>
+      <c r="B25" s="65">
         <v>8</v>
       </c>
-      <c r="C25" s="54"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="25" t="s">
+      <c r="C25" s="68"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
-      <c r="N25" s="25"/>
-      <c r="O25" s="25"/>
-      <c r="P25" s="25"/>
-      <c r="Q25" s="25"/>
-      <c r="R25" s="25"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="24"/>
+      <c r="Q25" s="24"/>
+      <c r="R25" s="24"/>
       <c r="S25" s="10"/>
-      <c r="T25" s="25"/>
-      <c r="U25" s="25"/>
+      <c r="T25" s="24"/>
+      <c r="U25" s="24"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="53"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="25" t="s">
+      <c r="A26" s="14"/>
+      <c r="B26" s="65"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="70"/>
+      <c r="F26" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="25"/>
-      <c r="N26" s="25"/>
-      <c r="O26" s="25"/>
-      <c r="P26" s="25"/>
-      <c r="Q26" s="25"/>
-      <c r="R26" s="25"/>
-      <c r="S26" s="25"/>
-      <c r="T26" s="25"/>
-      <c r="U26" s="25"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="24"/>
+      <c r="R26" s="24"/>
+      <c r="S26" s="24"/>
+      <c r="T26" s="24"/>
+      <c r="U26" s="24"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
-      <c r="B27" s="53">
+      <c r="A27" s="19"/>
+      <c r="B27" s="65">
         <v>9</v>
       </c>
-      <c r="C27" s="54"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="25" t="s">
+      <c r="C27" s="68"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="25"/>
-      <c r="N27" s="25"/>
-      <c r="O27" s="25"/>
-      <c r="P27" s="25"/>
-      <c r="Q27" s="25"/>
-      <c r="R27" s="25"/>
-      <c r="S27" s="25"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="24"/>
+      <c r="N27" s="24"/>
+      <c r="O27" s="24"/>
+      <c r="P27" s="24"/>
+      <c r="Q27" s="24"/>
+      <c r="R27" s="24"/>
+      <c r="S27" s="24"/>
       <c r="T27" s="10"/>
       <c r="U27" s="10"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="53"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="25" t="s">
+      <c r="A28" s="14"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
-      <c r="N28" s="25"/>
-      <c r="O28" s="25"/>
-      <c r="P28" s="25"/>
-      <c r="Q28" s="25"/>
-      <c r="R28" s="25"/>
-      <c r="S28" s="25"/>
-      <c r="T28" s="25"/>
-      <c r="U28" s="25"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="24"/>
+      <c r="Q28" s="24"/>
+      <c r="R28" s="24"/>
+      <c r="S28" s="24"/>
+      <c r="T28" s="24"/>
+      <c r="U28" s="24"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
-      <c r="B29" s="53">
+      <c r="A29" s="19"/>
+      <c r="B29" s="65">
         <v>10</v>
       </c>
-      <c r="C29" s="54"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="25" t="s">
+      <c r="C29" s="68"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="25"/>
-      <c r="N29" s="25"/>
-      <c r="O29" s="25"/>
-      <c r="P29" s="25"/>
-      <c r="Q29" s="25"/>
-      <c r="R29" s="25"/>
-      <c r="S29" s="25"/>
-      <c r="T29" s="25"/>
-      <c r="U29" s="25"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="24"/>
+      <c r="O29" s="24"/>
+      <c r="P29" s="24"/>
+      <c r="Q29" s="24"/>
+      <c r="R29" s="24"/>
+      <c r="S29" s="24"/>
+      <c r="T29" s="24"/>
+      <c r="U29" s="24"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="53"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="25" t="s">
+      <c r="A30" s="14"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="25"/>
-      <c r="K30" s="25"/>
-      <c r="L30" s="25"/>
-      <c r="M30" s="25"/>
-      <c r="N30" s="25"/>
-      <c r="O30" s="25"/>
-      <c r="P30" s="25"/>
-      <c r="Q30" s="25"/>
-      <c r="R30" s="25"/>
-      <c r="S30" s="25"/>
-      <c r="T30" s="25"/>
-      <c r="U30" s="25"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="24"/>
+      <c r="O30" s="24"/>
+      <c r="P30" s="24"/>
+      <c r="Q30" s="24"/>
+      <c r="R30" s="24"/>
+      <c r="S30" s="24"/>
+      <c r="T30" s="24"/>
+      <c r="U30" s="24"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
-      <c r="B31" s="53">
+      <c r="A31" s="19"/>
+      <c r="B31" s="65">
         <v>11</v>
       </c>
-      <c r="C31" s="54"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="25" t="s">
+      <c r="C31" s="68"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="25"/>
-      <c r="N31" s="25"/>
-      <c r="O31" s="25"/>
-      <c r="P31" s="25"/>
-      <c r="Q31" s="25"/>
-      <c r="R31" s="25"/>
-      <c r="S31" s="25"/>
-      <c r="T31" s="25"/>
-      <c r="U31" s="25"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
+      <c r="N31" s="24"/>
+      <c r="O31" s="24"/>
+      <c r="P31" s="24"/>
+      <c r="Q31" s="24"/>
+      <c r="R31" s="24"/>
+      <c r="S31" s="24"/>
+      <c r="T31" s="24"/>
+      <c r="U31" s="24"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="53"/>
-      <c r="C32" s="54"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="25" t="s">
+      <c r="A32" s="14"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="67"/>
+      <c r="E32" s="70"/>
+      <c r="F32" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="25"/>
-      <c r="N32" s="25"/>
-      <c r="O32" s="25"/>
-      <c r="P32" s="25"/>
-      <c r="Q32" s="25"/>
-      <c r="R32" s="25"/>
-      <c r="S32" s="25"/>
-      <c r="T32" s="25"/>
-      <c r="U32" s="25"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="24"/>
+      <c r="P32" s="24"/>
+      <c r="Q32" s="24"/>
+      <c r="R32" s="24"/>
+      <c r="S32" s="24"/>
+      <c r="T32" s="24"/>
+      <c r="U32" s="24"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
-      <c r="B33" s="53">
+      <c r="A33" s="19"/>
+      <c r="B33" s="65">
         <v>12</v>
       </c>
-      <c r="C33" s="54"/>
-      <c r="D33" s="55"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="25" t="s">
+      <c r="C33" s="68"/>
+      <c r="D33" s="67"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="25"/>
-      <c r="N33" s="25"/>
-      <c r="O33" s="25"/>
-      <c r="P33" s="25"/>
-      <c r="Q33" s="25"/>
-      <c r="R33" s="25"/>
-      <c r="S33" s="25"/>
-      <c r="T33" s="25"/>
-      <c r="U33" s="25"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="24"/>
+      <c r="P33" s="24"/>
+      <c r="Q33" s="24"/>
+      <c r="R33" s="24"/>
+      <c r="S33" s="24"/>
+      <c r="T33" s="24"/>
+      <c r="U33" s="24"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="B34" s="53"/>
-      <c r="C34" s="54"/>
-      <c r="D34" s="55"/>
-      <c r="E34" s="57"/>
-      <c r="F34" s="25" t="s">
+      <c r="A34" s="14"/>
+      <c r="B34" s="65"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
-      <c r="L34" s="25"/>
-      <c r="M34" s="25"/>
-      <c r="N34" s="25"/>
-      <c r="O34" s="25"/>
-      <c r="P34" s="25"/>
-      <c r="Q34" s="25"/>
-      <c r="R34" s="25"/>
-      <c r="S34" s="25"/>
-      <c r="T34" s="25"/>
-      <c r="U34" s="25"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="24"/>
+      <c r="N34" s="24"/>
+      <c r="O34" s="24"/>
+      <c r="P34" s="24"/>
+      <c r="Q34" s="24"/>
+      <c r="R34" s="24"/>
+      <c r="S34" s="24"/>
+      <c r="T34" s="24"/>
+      <c r="U34" s="24"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
-      <c r="B35" s="53">
+      <c r="A35" s="19"/>
+      <c r="B35" s="65">
         <v>13</v>
       </c>
-      <c r="C35" s="54"/>
-      <c r="D35" s="55"/>
-      <c r="E35" s="56"/>
-      <c r="F35" s="25" t="s">
+      <c r="C35" s="68"/>
+      <c r="D35" s="67"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="25"/>
-      <c r="N35" s="25"/>
-      <c r="O35" s="25"/>
-      <c r="P35" s="25"/>
-      <c r="Q35" s="25"/>
-      <c r="R35" s="25"/>
-      <c r="S35" s="25"/>
-      <c r="T35" s="25"/>
-      <c r="U35" s="25"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="24"/>
+      <c r="N35" s="24"/>
+      <c r="O35" s="24"/>
+      <c r="P35" s="24"/>
+      <c r="Q35" s="24"/>
+      <c r="R35" s="24"/>
+      <c r="S35" s="24"/>
+      <c r="T35" s="24"/>
+      <c r="U35" s="24"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="53"/>
-      <c r="C36" s="54"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="25" t="s">
+      <c r="A36" s="14"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="68"/>
+      <c r="D36" s="67"/>
+      <c r="E36" s="70"/>
+      <c r="F36" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
-      <c r="L36" s="25"/>
-      <c r="M36" s="25"/>
-      <c r="N36" s="25"/>
-      <c r="O36" s="25"/>
-      <c r="P36" s="25"/>
-      <c r="Q36" s="25"/>
-      <c r="R36" s="25"/>
-      <c r="S36" s="25"/>
-      <c r="T36" s="25"/>
-      <c r="U36" s="25"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="24"/>
+      <c r="L36" s="24"/>
+      <c r="M36" s="24"/>
+      <c r="N36" s="24"/>
+      <c r="O36" s="24"/>
+      <c r="P36" s="24"/>
+      <c r="Q36" s="24"/>
+      <c r="R36" s="24"/>
+      <c r="S36" s="24"/>
+      <c r="T36" s="24"/>
+      <c r="U36" s="24"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
-      <c r="B37" s="53">
+      <c r="A37" s="19"/>
+      <c r="B37" s="65">
         <v>14</v>
       </c>
-      <c r="C37" s="54"/>
-      <c r="D37" s="55"/>
-      <c r="E37" s="56"/>
-      <c r="F37" s="25" t="s">
+      <c r="C37" s="68"/>
+      <c r="D37" s="67"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
-      <c r="L37" s="25"/>
-      <c r="M37" s="25"/>
-      <c r="N37" s="25"/>
-      <c r="O37" s="25"/>
-      <c r="P37" s="25"/>
-      <c r="Q37" s="25"/>
-      <c r="R37" s="25"/>
-      <c r="S37" s="25"/>
-      <c r="T37" s="25"/>
-      <c r="U37" s="25"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
+      <c r="L37" s="24"/>
+      <c r="M37" s="24"/>
+      <c r="N37" s="24"/>
+      <c r="O37" s="24"/>
+      <c r="P37" s="24"/>
+      <c r="Q37" s="24"/>
+      <c r="R37" s="24"/>
+      <c r="S37" s="24"/>
+      <c r="T37" s="24"/>
+      <c r="U37" s="24"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="53"/>
-      <c r="C38" s="54"/>
-      <c r="D38" s="55"/>
-      <c r="E38" s="57"/>
-      <c r="F38" s="25" t="s">
+      <c r="A38" s="14"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="68"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="70"/>
+      <c r="F38" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="25"/>
-      <c r="L38" s="25"/>
-      <c r="M38" s="25"/>
-      <c r="N38" s="25"/>
-      <c r="O38" s="25"/>
-      <c r="P38" s="25"/>
-      <c r="Q38" s="25"/>
-      <c r="R38" s="25"/>
-      <c r="S38" s="25"/>
-      <c r="T38" s="25"/>
-      <c r="U38" s="25"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24"/>
+      <c r="K38" s="24"/>
+      <c r="L38" s="24"/>
+      <c r="M38" s="24"/>
+      <c r="N38" s="24"/>
+      <c r="O38" s="24"/>
+      <c r="P38" s="24"/>
+      <c r="Q38" s="24"/>
+      <c r="R38" s="24"/>
+      <c r="S38" s="24"/>
+      <c r="T38" s="24"/>
+      <c r="U38" s="24"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="20"/>
-      <c r="B39" s="53">
+      <c r="A39" s="19"/>
+      <c r="B39" s="65">
         <v>15</v>
       </c>
-      <c r="C39" s="54"/>
-      <c r="D39" s="55"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="25" t="s">
+      <c r="C39" s="68"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="G39" s="25"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="25"/>
-      <c r="L39" s="25"/>
-      <c r="M39" s="25"/>
-      <c r="N39" s="25"/>
-      <c r="O39" s="25"/>
-      <c r="P39" s="25"/>
-      <c r="Q39" s="25"/>
-      <c r="R39" s="25"/>
-      <c r="S39" s="25"/>
-      <c r="T39" s="25"/>
-      <c r="U39" s="25"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24"/>
+      <c r="K39" s="24"/>
+      <c r="L39" s="24"/>
+      <c r="M39" s="24"/>
+      <c r="N39" s="24"/>
+      <c r="O39" s="24"/>
+      <c r="P39" s="24"/>
+      <c r="Q39" s="24"/>
+      <c r="R39" s="24"/>
+      <c r="S39" s="24"/>
+      <c r="T39" s="24"/>
+      <c r="U39" s="24"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="B40" s="53"/>
-      <c r="C40" s="54"/>
-      <c r="D40" s="55"/>
-      <c r="E40" s="57"/>
-      <c r="F40" s="25" t="s">
+      <c r="A40" s="14"/>
+      <c r="B40" s="65"/>
+      <c r="C40" s="68"/>
+      <c r="D40" s="67"/>
+      <c r="E40" s="70"/>
+      <c r="F40" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25"/>
-      <c r="L40" s="25"/>
-      <c r="M40" s="25"/>
-      <c r="N40" s="25"/>
-      <c r="O40" s="25"/>
-      <c r="P40" s="25"/>
-      <c r="Q40" s="25"/>
-      <c r="R40" s="25"/>
-      <c r="S40" s="25"/>
-      <c r="T40" s="25"/>
-      <c r="U40" s="25"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
+      <c r="K40" s="24"/>
+      <c r="L40" s="24"/>
+      <c r="M40" s="24"/>
+      <c r="N40" s="24"/>
+      <c r="O40" s="24"/>
+      <c r="P40" s="24"/>
+      <c r="Q40" s="24"/>
+      <c r="R40" s="24"/>
+      <c r="S40" s="24"/>
+      <c r="T40" s="24"/>
+      <c r="U40" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="E13:E14"/>
     <mergeCell ref="B2:U4"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
@@ -3750,51 +3894,6 @@
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="G9:U9"/>
     <mergeCell ref="P6:U6"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:D38"/>
-    <mergeCell ref="E37:E38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3813,198 +3912,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="14"/>
       <c r="D3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="15"/>
+      <c r="E3" s="14"/>
       <c r="F3" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="27" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="27" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="27" t="s">
+      <c r="E4" s="14"/>
+      <c r="F4" s="26" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15" t="s">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15" t="s">
+      <c r="E5" s="14"/>
+      <c r="F5" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15" t="s">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15" t="s">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15" t="s">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15" t="s">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15" t="s">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
jdre-06/04/2015-Se anexo BITACORA.xlsx correspondiente a la semana 12
</commit_message>
<xml_diff>
--- a/ afgmx/AFGMX/ADMON_DEL_PROYECTO/BITACORAS/2015/CUAT_1_ENER_ABR/PARCIAL_3/BITACORA.xlsx
+++ b/ afgmx/AFGMX/ADMON_DEL_PROYECTO/BITACORAS/2015/CUAT_1_ENER_ABR/PARCIAL_3/BITACORA.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diegox\Desktop\Proyecto\AFGMX\ADMON_DEL_PROYECTO\BITACORAS\2015\CUAT_1_ENER_ABR\PARCIAL_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\AFG\AFGMX\ADMON_DEL_PROYECTO\BITACORAS\2015\CUAT_1_ENER_ABR\PARCIAL_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="19440" windowHeight="8340" activeTab="2"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="19440" windowHeight="8340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="88">
   <si>
     <t>UNIVERSIDAD TECNOLÓGICA DEL  CENTRO DE VERACRUZ
 TECNOLOGÍAS DE LA INFORMACIÓN Y COMUNICACIÓN
@@ -261,6 +261,39 @@
   </si>
   <si>
     <t>Biacora</t>
+  </si>
+  <si>
+    <t>Verificacion de artefacros de acorde al plan</t>
+  </si>
+  <si>
+    <t>Jose Carlos Vazquez Garcia</t>
+  </si>
+  <si>
+    <t>Creacion del plan de pruebas</t>
+  </si>
+  <si>
+    <t>Toma de decisiones por parte del equipo de desarrollo</t>
+  </si>
+  <si>
+    <t>Se llego al acuerdo de cual seria el plan para continuar con el desarrollo del proyecto</t>
+  </si>
+  <si>
+    <t>Bitácora</t>
+  </si>
+  <si>
+    <t>Investigación de hosting</t>
+  </si>
+  <si>
+    <t>Ricardo Navarrete Crisanto</t>
+  </si>
+  <si>
+    <t>Cotización_de_precios</t>
+  </si>
+  <si>
+    <t>Integracion_del_plan_de_pruebas</t>
+  </si>
+  <si>
+    <t>Se llevo a cabo  la  busqueda de diversos sitios que ofertan los servicios de dominio y hosting para poner en linea el proyecto, así como determinar posteriormente cual sera el mas adecuado..</t>
   </si>
 </sst>
 </file>
@@ -1276,7 +1309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1347,6 +1380,42 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="52" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="22" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1365,27 +1434,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="22" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1395,6 +1443,24 @@
     <xf numFmtId="0" fontId="52" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1434,38 +1500,8 @@
     <xf numFmtId="15" fontId="53" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="52" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="52" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1986,46 +2022,46 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="38"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="50"/>
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="38"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="50"/>
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="38"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="50"/>
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2048,13 +2084,13 @@
       <c r="C6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
@@ -2066,13 +2102,13 @@
       <c r="C7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
@@ -2084,13 +2120,13 @@
       <c r="C8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
       <c r="K8" s="14"/>
@@ -2102,13 +2138,13 @@
       <c r="C9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
@@ -2120,13 +2156,13 @@
       <c r="C10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="42">
+      <c r="D10" s="43">
         <v>1</v>
       </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
@@ -2138,13 +2174,13 @@
       <c r="C11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
@@ -2170,11 +2206,11 @@
       <c r="C13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
@@ -2186,13 +2222,13 @@
       <c r="C14" s="25">
         <v>1</v>
       </c>
-      <c r="D14" s="47" t="s">
+      <c r="D14" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
       <c r="K14" s="14"/>
@@ -2204,13 +2240,13 @@
       <c r="C15" s="25">
         <v>2</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
@@ -2222,13 +2258,13 @@
       <c r="C16" s="25">
         <v>3</v>
       </c>
-      <c r="D16" s="43" t="s">
+      <c r="D16" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
@@ -2240,13 +2276,13 @@
       <c r="C17" s="25">
         <v>4</v>
       </c>
-      <c r="D17" s="43" t="s">
+      <c r="D17" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
@@ -2258,13 +2294,13 @@
       <c r="C18" s="25">
         <v>5</v>
       </c>
-      <c r="D18" s="43" t="s">
+      <c r="D18" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
       <c r="K18" s="14"/>
@@ -2276,11 +2312,11 @@
       <c r="C19" s="25">
         <v>6</v>
       </c>
-      <c r="D19" s="43"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
       <c r="K19" s="14"/>
@@ -2302,6 +2338,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B2:K4"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="D9:H9"/>
     <mergeCell ref="D16:H16"/>
     <mergeCell ref="D17:H17"/>
     <mergeCell ref="D18:H18"/>
@@ -2311,11 +2352,6 @@
     <mergeCell ref="D13:H13"/>
     <mergeCell ref="D14:H14"/>
     <mergeCell ref="D15:H15"/>
-    <mergeCell ref="B2:K4"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="D9:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2326,8 +2362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="E9" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2371,42 +2407,42 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="51"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="56"/>
       <c r="J3" s="18"/>
       <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="51"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="56"/>
       <c r="J4" s="18"/>
       <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="51"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="56"/>
       <c r="J5" s="18"/>
       <c r="K5" s="7"/>
     </row>
@@ -2470,7 +2506,7 @@
       <c r="B9" s="32">
         <v>10</v>
       </c>
-      <c r="C9" s="71">
+      <c r="C9" s="36">
         <v>42074</v>
       </c>
       <c r="D9" s="31" t="s">
@@ -2500,7 +2536,7 @@
       <c r="C10" s="34">
         <v>42074</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="D10" s="38" t="s">
         <v>56</v>
       </c>
       <c r="E10" s="32" t="s">
@@ -2527,7 +2563,7 @@
       <c r="C11" s="34">
         <v>42081</v>
       </c>
-      <c r="D11" s="73" t="s">
+      <c r="D11" s="38" t="s">
         <v>64</v>
       </c>
       <c r="E11" s="32" t="s">
@@ -2554,7 +2590,7 @@
       <c r="C12" s="34">
         <v>42081</v>
       </c>
-      <c r="D12" s="74" t="s">
+      <c r="D12" s="39" t="s">
         <v>66</v>
       </c>
       <c r="E12" s="32" t="s">
@@ -2569,7 +2605,7 @@
       <c r="H12" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="I12" s="72"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="2"/>
       <c r="K12" s="14"/>
     </row>
@@ -2596,7 +2632,7 @@
       <c r="H13" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="I13" s="72"/>
+      <c r="I13" s="37"/>
       <c r="J13" s="2"/>
       <c r="K13" s="14"/>
     </row>
@@ -2608,7 +2644,7 @@
       <c r="C14" s="34">
         <v>42081</v>
       </c>
-      <c r="D14" s="75" t="s">
+      <c r="D14" s="40" t="s">
         <v>71</v>
       </c>
       <c r="E14" s="32" t="s">
@@ -2623,7 +2659,7 @@
       <c r="H14" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="I14" s="72"/>
+      <c r="I14" s="37"/>
       <c r="J14" s="2"/>
       <c r="K14" s="14"/>
     </row>
@@ -2635,7 +2671,7 @@
       <c r="C15" s="34">
         <v>42081</v>
       </c>
-      <c r="D15" s="73" t="s">
+      <c r="D15" s="38" t="s">
         <v>74</v>
       </c>
       <c r="E15" s="32" t="s">
@@ -2650,45 +2686,87 @@
       <c r="H15" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="I15" s="72"/>
+      <c r="I15" s="37"/>
       <c r="J15" s="2"/>
       <c r="K15" s="14"/>
     </row>
     <row r="16" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
+      <c r="B16" s="32">
+        <v>12</v>
+      </c>
+      <c r="C16" s="76">
+        <v>42096</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="H16" s="27" t="s">
+        <v>78</v>
+      </c>
       <c r="I16" s="12"/>
       <c r="J16" s="2"/>
       <c r="K16" s="14"/>
     </row>
     <row r="17" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
+      <c r="B17" s="32">
+        <v>12</v>
+      </c>
+      <c r="C17" s="76">
+        <v>42096</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="H17" s="27" t="s">
+        <v>62</v>
+      </c>
       <c r="I17" s="12"/>
       <c r="J17" s="2"/>
       <c r="K17" s="14"/>
     </row>
     <row r="18" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
+      <c r="B18" s="32">
+        <v>12</v>
+      </c>
+      <c r="C18" s="76">
+        <v>42096</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" s="27" t="s">
+        <v>84</v>
+      </c>
       <c r="I18" s="12"/>
       <c r="J18" s="2"/>
       <c r="K18" s="14"/>
@@ -2762,7 +2840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
@@ -2801,74 +2879,74 @@
     </row>
     <row r="2" spans="1:21" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="54"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="64"/>
+      <c r="R2" s="64"/>
+      <c r="S2" s="64"/>
+      <c r="T2" s="64"/>
+      <c r="U2" s="65"/>
     </row>
     <row r="3" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
-      <c r="B3" s="52"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="53"/>
-      <c r="S3" s="53"/>
-      <c r="T3" s="53"/>
-      <c r="U3" s="54"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="64"/>
+      <c r="T3" s="64"/>
+      <c r="U3" s="65"/>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="53"/>
-      <c r="M4" s="53"/>
-      <c r="N4" s="53"/>
-      <c r="O4" s="53"/>
-      <c r="P4" s="53"/>
-      <c r="Q4" s="53"/>
-      <c r="R4" s="53"/>
-      <c r="S4" s="53"/>
-      <c r="T4" s="53"/>
-      <c r="U4" s="54"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="64"/>
+      <c r="N4" s="64"/>
+      <c r="O4" s="64"/>
+      <c r="P4" s="64"/>
+      <c r="Q4" s="64"/>
+      <c r="R4" s="64"/>
+      <c r="S4" s="64"/>
+      <c r="T4" s="64"/>
+      <c r="U4" s="65"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
@@ -2895,10 +2973,10 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="55"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="35" t="s">
         <v>63</v>
       </c>
@@ -2915,21 +2993,21 @@
       <c r="M6" s="14"/>
       <c r="N6" s="14"/>
       <c r="O6" s="14"/>
-      <c r="P6" s="64">
+      <c r="P6" s="75">
         <v>42074</v>
       </c>
-      <c r="Q6" s="64"/>
-      <c r="R6" s="64"/>
-      <c r="S6" s="64"/>
-      <c r="T6" s="64"/>
-      <c r="U6" s="64"/>
+      <c r="Q6" s="75"/>
+      <c r="R6" s="75"/>
+      <c r="S6" s="75"/>
+      <c r="T6" s="75"/>
+      <c r="U6" s="75"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="55"/>
+      <c r="C7" s="66"/>
       <c r="D7" s="30"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -2974,44 +3052,44 @@
     </row>
     <row r="9" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="57"/>
-      <c r="E9" s="58" t="s">
+      <c r="D9" s="68"/>
+      <c r="E9" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="59" t="s">
+      <c r="F9" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="61" t="s">
+      <c r="G9" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="62"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="62"/>
-      <c r="K9" s="62"/>
-      <c r="L9" s="62"/>
-      <c r="M9" s="62"/>
-      <c r="N9" s="62"/>
-      <c r="O9" s="62"/>
-      <c r="P9" s="62"/>
-      <c r="Q9" s="62"/>
-      <c r="R9" s="62"/>
-      <c r="S9" s="62"/>
-      <c r="T9" s="62"/>
-      <c r="U9" s="63"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="73"/>
+      <c r="N9" s="73"/>
+      <c r="O9" s="73"/>
+      <c r="P9" s="73"/>
+      <c r="Q9" s="73"/>
+      <c r="R9" s="73"/>
+      <c r="S9" s="73"/>
+      <c r="T9" s="73"/>
+      <c r="U9" s="74"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="60"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="71"/>
       <c r="G10" s="22">
         <v>1</v>
       </c>
@@ -3060,12 +3138,12 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
-      <c r="B11" s="65">
+      <c r="B11" s="57">
         <v>1</v>
       </c>
-      <c r="C11" s="66"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="69"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="60"/>
       <c r="F11" s="24" t="s">
         <v>27</v>
       </c>
@@ -3087,10 +3165,10 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="67"/>
-      <c r="E12" s="70"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="61"/>
       <c r="F12" s="24" t="s">
         <v>28</v>
       </c>
@@ -3112,12 +3190,12 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
-      <c r="B13" s="65">
+      <c r="B13" s="57">
         <v>2</v>
       </c>
-      <c r="C13" s="68"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="69"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="60"/>
       <c r="F13" s="24" t="s">
         <v>27</v>
       </c>
@@ -3139,10 +3217,10 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
-      <c r="B14" s="65"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="70"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="61"/>
       <c r="F14" s="24" t="s">
         <v>28</v>
       </c>
@@ -3164,12 +3242,12 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
-      <c r="B15" s="65">
+      <c r="B15" s="57">
         <v>3</v>
       </c>
-      <c r="C15" s="66"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="69"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="60"/>
       <c r="F15" s="24" t="s">
         <v>27</v>
       </c>
@@ -3191,10 +3269,10 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="70"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="61"/>
       <c r="F16" s="24" t="s">
         <v>28</v>
       </c>
@@ -3216,12 +3294,12 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
-      <c r="B17" s="65">
+      <c r="B17" s="57">
         <v>4</v>
       </c>
-      <c r="C17" s="66"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="69"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="60"/>
       <c r="F17" s="24" t="s">
         <v>27</v>
       </c>
@@ -3243,10 +3321,10 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
-      <c r="B18" s="65"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="70"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="61"/>
       <c r="F18" s="24" t="s">
         <v>28</v>
       </c>
@@ -3268,12 +3346,12 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
-      <c r="B19" s="65">
+      <c r="B19" s="57">
         <v>5</v>
       </c>
-      <c r="C19" s="68"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="69"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="60"/>
       <c r="F19" s="24" t="s">
         <v>27</v>
       </c>
@@ -3295,10 +3373,10 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
-      <c r="B20" s="65"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="70"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="61"/>
       <c r="F20" s="24" t="s">
         <v>28</v>
       </c>
@@ -3320,12 +3398,12 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
-      <c r="B21" s="65">
+      <c r="B21" s="57">
         <v>6</v>
       </c>
-      <c r="C21" s="66"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="69"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="60"/>
       <c r="F21" s="24" t="s">
         <v>27</v>
       </c>
@@ -3347,10 +3425,10 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
-      <c r="B22" s="65"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="70"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="61"/>
       <c r="F22" s="24" t="s">
         <v>28</v>
       </c>
@@ -3372,12 +3450,12 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
-      <c r="B23" s="65">
+      <c r="B23" s="57">
         <v>7</v>
       </c>
-      <c r="C23" s="68"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="69"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="60"/>
       <c r="F23" s="24" t="s">
         <v>27</v>
       </c>
@@ -3399,10 +3477,10 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
-      <c r="B24" s="65"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="70"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="61"/>
       <c r="F24" s="24" t="s">
         <v>28</v>
       </c>
@@ -3424,12 +3502,12 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
-      <c r="B25" s="65">
+      <c r="B25" s="57">
         <v>8</v>
       </c>
-      <c r="C25" s="68"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="69"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="60"/>
       <c r="F25" s="24" t="s">
         <v>27</v>
       </c>
@@ -3451,10 +3529,10 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
-      <c r="B26" s="65"/>
-      <c r="C26" s="68"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="70"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="61"/>
       <c r="F26" s="24" t="s">
         <v>28</v>
       </c>
@@ -3476,12 +3554,12 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
-      <c r="B27" s="65">
+      <c r="B27" s="57">
         <v>9</v>
       </c>
-      <c r="C27" s="68"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="69"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="60"/>
       <c r="F27" s="24" t="s">
         <v>27</v>
       </c>
@@ -3503,10 +3581,10 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
-      <c r="B28" s="65"/>
-      <c r="C28" s="68"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="70"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="61"/>
       <c r="F28" s="24" t="s">
         <v>28</v>
       </c>
@@ -3528,12 +3606,12 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
-      <c r="B29" s="65">
+      <c r="B29" s="57">
         <v>10</v>
       </c>
-      <c r="C29" s="68"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="69"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="60"/>
       <c r="F29" s="24" t="s">
         <v>27</v>
       </c>
@@ -3555,10 +3633,10 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
-      <c r="B30" s="65"/>
-      <c r="C30" s="68"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="70"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="61"/>
       <c r="F30" s="24" t="s">
         <v>28</v>
       </c>
@@ -3580,12 +3658,12 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
-      <c r="B31" s="65">
+      <c r="B31" s="57">
         <v>11</v>
       </c>
-      <c r="C31" s="68"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="69"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="60"/>
       <c r="F31" s="24" t="s">
         <v>27</v>
       </c>
@@ -3607,10 +3685,10 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
-      <c r="B32" s="65"/>
-      <c r="C32" s="68"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="70"/>
+      <c r="B32" s="57"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="61"/>
       <c r="F32" s="24" t="s">
         <v>28</v>
       </c>
@@ -3632,12 +3710,12 @@
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="19"/>
-      <c r="B33" s="65">
+      <c r="B33" s="57">
         <v>12</v>
       </c>
-      <c r="C33" s="68"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="69"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="60"/>
       <c r="F33" s="24" t="s">
         <v>27</v>
       </c>
@@ -3659,10 +3737,10 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
-      <c r="B34" s="65"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="67"/>
-      <c r="E34" s="70"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="61"/>
       <c r="F34" s="24" t="s">
         <v>28</v>
       </c>
@@ -3684,12 +3762,12 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="19"/>
-      <c r="B35" s="65">
+      <c r="B35" s="57">
         <v>13</v>
       </c>
-      <c r="C35" s="68"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="69"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="60"/>
       <c r="F35" s="24" t="s">
         <v>27</v>
       </c>
@@ -3711,10 +3789,10 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
-      <c r="B36" s="65"/>
-      <c r="C36" s="68"/>
-      <c r="D36" s="67"/>
-      <c r="E36" s="70"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="61"/>
       <c r="F36" s="24" t="s">
         <v>28</v>
       </c>
@@ -3736,12 +3814,12 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="19"/>
-      <c r="B37" s="65">
+      <c r="B37" s="57">
         <v>14</v>
       </c>
-      <c r="C37" s="68"/>
-      <c r="D37" s="67"/>
-      <c r="E37" s="69"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="59"/>
+      <c r="E37" s="60"/>
       <c r="F37" s="24" t="s">
         <v>27</v>
       </c>
@@ -3763,10 +3841,10 @@
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
-      <c r="B38" s="65"/>
-      <c r="C38" s="68"/>
-      <c r="D38" s="67"/>
-      <c r="E38" s="70"/>
+      <c r="B38" s="57"/>
+      <c r="C38" s="58"/>
+      <c r="D38" s="59"/>
+      <c r="E38" s="61"/>
       <c r="F38" s="24" t="s">
         <v>28</v>
       </c>
@@ -3788,12 +3866,12 @@
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="19"/>
-      <c r="B39" s="65">
+      <c r="B39" s="57">
         <v>15</v>
       </c>
-      <c r="C39" s="68"/>
-      <c r="D39" s="67"/>
-      <c r="E39" s="69"/>
+      <c r="C39" s="58"/>
+      <c r="D39" s="59"/>
+      <c r="E39" s="60"/>
       <c r="F39" s="24" t="s">
         <v>27</v>
       </c>
@@ -3815,10 +3893,10 @@
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="14"/>
-      <c r="B40" s="65"/>
-      <c r="C40" s="68"/>
-      <c r="D40" s="67"/>
-      <c r="E40" s="70"/>
+      <c r="B40" s="57"/>
+      <c r="C40" s="58"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="61"/>
       <c r="F40" s="24" t="s">
         <v>28</v>
       </c>
@@ -3840,6 +3918,51 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="B2:U4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:U9"/>
+    <mergeCell ref="P6:U6"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:D34"/>
+    <mergeCell ref="E33:E34"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="C39:D40"/>
     <mergeCell ref="E39:E40"/>
@@ -3849,51 +3972,6 @@
     <mergeCell ref="B37:B38"/>
     <mergeCell ref="C37:D38"/>
     <mergeCell ref="E37:E38"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="B2:U4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:U9"/>
-    <mergeCell ref="P6:U6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
jdre-08/04/2015-Se actualiza la BITACORA.xlsx con la actividad realizada y se anexa el archivo FACTURA.pdf que respalda dicha actividad.
</commit_message>
<xml_diff>
--- a/ afgmx/AFGMX/ADMON_DEL_PROYECTO/BITACORAS/2015/CUAT_1_ENER_ABR/PARCIAL_3/BITACORA.xlsx
+++ b/ afgmx/AFGMX/ADMON_DEL_PROYECTO/BITACORAS/2015/CUAT_1_ENER_ABR/PARCIAL_3/BITACORA.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="83">
   <si>
     <t>UNIVERSIDAD TECNOLÓGICA DEL  CENTRO DE VERACRUZ
 TECNOLOGÍAS DE LA INFORMACIÓN Y COMUNICACIÓN
@@ -267,6 +267,15 @@
   </si>
   <si>
     <t>CRONOGRAMA_AFGMX</t>
+  </si>
+  <si>
+    <t>Pago de servicio de hosting</t>
+  </si>
+  <si>
+    <t>Se anexa la factura del pago de hosting que se realizo para obtener el dominio para la aplicación web</t>
+  </si>
+  <si>
+    <t>FACTURA.pdf</t>
   </si>
 </sst>
 </file>
@@ -924,6 +933,27 @@
     <xf numFmtId="14" fontId="29" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -940,27 +970,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1422,46 +1431,46 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="36"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="43"/>
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="36"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="43"/>
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="36"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="43"/>
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1484,13 +1493,13 @@
       <c r="C6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
@@ -1502,13 +1511,13 @@
       <c r="C7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
@@ -1520,13 +1529,13 @@
       <c r="C8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
@@ -1538,13 +1547,13 @@
       <c r="C9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
@@ -1556,13 +1565,13 @@
       <c r="C10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="40">
+      <c r="D10" s="36">
         <v>1</v>
       </c>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
@@ -1574,13 +1583,13 @@
       <c r="C11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
@@ -1606,11 +1615,11 @@
       <c r="C13" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
@@ -1622,13 +1631,13 @@
       <c r="C14" s="19">
         <v>1</v>
       </c>
-      <c r="D14" s="45" t="s">
+      <c r="D14" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
@@ -1640,13 +1649,13 @@
       <c r="C15" s="19">
         <v>2</v>
       </c>
-      <c r="D15" s="41" t="s">
+      <c r="D15" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
@@ -1658,13 +1667,13 @@
       <c r="C16" s="19">
         <v>3</v>
       </c>
-      <c r="D16" s="41" t="s">
+      <c r="D16" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
@@ -1676,13 +1685,13 @@
       <c r="C17" s="19">
         <v>4</v>
       </c>
-      <c r="D17" s="41" t="s">
+      <c r="D17" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
@@ -1694,13 +1703,13 @@
       <c r="C18" s="19">
         <v>5</v>
       </c>
-      <c r="D18" s="41" t="s">
+      <c r="D18" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
@@ -1712,11 +1721,11 @@
       <c r="C19" s="19">
         <v>6</v>
       </c>
-      <c r="D19" s="41"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
@@ -1738,6 +1747,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B2:K4"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="D9:H9"/>
     <mergeCell ref="D16:H16"/>
     <mergeCell ref="D17:H17"/>
     <mergeCell ref="D18:H18"/>
@@ -1747,11 +1761,6 @@
     <mergeCell ref="D13:H13"/>
     <mergeCell ref="D14:H14"/>
     <mergeCell ref="D15:H15"/>
-    <mergeCell ref="B2:K4"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="D9:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1762,8 +1771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G9" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2200,13 +2209,27 @@
     </row>
     <row r="20" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
+      <c r="B20" s="25">
+        <v>13</v>
+      </c>
+      <c r="C20" s="33">
+        <v>42102</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>62</v>
+      </c>
       <c r="I20" s="10"/>
       <c r="J20" s="2"/>
       <c r="K20" s="12"/>

</xml_diff>